<commit_message>
Added tables through simple SCM formulas
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/Table1-KdValuesAndMineralProp.xlsx
+++ b/Manuscript/Tables/Table1-KdValuesAndMineralProp.xlsx
@@ -502,11 +502,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="203079000"/>
-        <c:axId val="203082136"/>
+        <c:axId val="84272560"/>
+        <c:axId val="212167608"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="203079000"/>
+        <c:axId val="84272560"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -563,12 +563,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203082136"/>
+        <c:crossAx val="212167608"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="203082136"/>
+        <c:axId val="212167608"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -625,7 +625,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="203079000"/>
+        <c:crossAx val="84272560"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1531,17 +1531,17 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I3" sqref="I3"/>
+      <selection activeCell="B18" sqref="B18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="28.625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="25.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="21.75" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="28.5703125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="25.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21.7109375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="9" customWidth="1"/>
-    <col min="6" max="6" width="27.25" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="23.125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="27.28515625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="26.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:9" x14ac:dyDescent="0.25">
@@ -1602,7 +1602,7 @@
         <v>382.9</v>
       </c>
       <c r="H3" s="10">
-        <f>E3/G3</f>
+        <f t="shared" ref="H3:H8" si="0">E3/G3</f>
         <v>0.60039174719247845</v>
       </c>
     </row>
@@ -1630,7 +1630,7 @@
         <v>382.9</v>
       </c>
       <c r="H4" s="10">
-        <f>E4/G4</f>
+        <f t="shared" si="0"/>
         <v>1.2310524941237921</v>
       </c>
     </row>
@@ -1658,7 +1658,7 @@
         <v>382.9</v>
       </c>
       <c r="H5" s="10">
-        <f>E5/G5</f>
+        <f t="shared" si="0"/>
         <v>6.4948550535387835</v>
       </c>
     </row>
@@ -1686,7 +1686,7 @@
         <v>382.9</v>
       </c>
       <c r="H6" s="10">
-        <f>E6/G6</f>
+        <f t="shared" si="0"/>
         <v>302.77539827631239</v>
       </c>
     </row>
@@ -1714,7 +1714,7 @@
         <v>253</v>
       </c>
       <c r="H7" s="9">
-        <f>E7/G7</f>
+        <f t="shared" si="0"/>
         <v>6.0671936758893281</v>
       </c>
     </row>
@@ -1742,7 +1742,7 @@
         <v>245</v>
       </c>
       <c r="H8" s="9">
-        <f>E8/G8</f>
+        <f t="shared" si="0"/>
         <v>5.8776816326530605</v>
       </c>
     </row>
@@ -2091,7 +2091,7 @@
         <v>6.8500000000000005E-2</v>
       </c>
       <c r="H21" s="10">
-        <f>E21/G21</f>
+        <f t="shared" ref="H21:H28" si="1">E21/G21</f>
         <v>7824.8175182481746</v>
       </c>
     </row>
@@ -2120,7 +2120,7 @@
         <v>6.8500000000000005E-2</v>
       </c>
       <c r="H22" s="10">
-        <f>E22/G22</f>
+        <f t="shared" si="1"/>
         <v>7591.2408759124082</v>
       </c>
     </row>
@@ -2148,7 +2148,7 @@
         <v>97.42</v>
       </c>
       <c r="H23" s="9">
-        <f>E23/G23</f>
+        <f t="shared" si="1"/>
         <v>38.226236912338329</v>
       </c>
       <c r="I23" t="s">
@@ -2179,7 +2179,7 @@
         <v>50.161999999999999</v>
       </c>
       <c r="H24" s="10">
-        <f>E24/G24</f>
+        <f t="shared" si="1"/>
         <v>134.36764881783023</v>
       </c>
     </row>
@@ -2207,7 +2207,7 @@
         <v>50.161999999999999</v>
       </c>
       <c r="H25" s="10">
-        <f>E25/G25</f>
+        <f t="shared" si="1"/>
         <v>353.8413540129979</v>
       </c>
     </row>
@@ -2235,7 +2235,7 @@
         <v>50.161999999999999</v>
       </c>
       <c r="H26" s="10">
-        <f>E26/G26</f>
+        <f t="shared" si="1"/>
         <v>428.07842590008374</v>
       </c>
     </row>
@@ -2263,7 +2263,7 @@
         <v>50.161999999999999</v>
       </c>
       <c r="H27" s="10">
-        <f>E27/G27</f>
+        <f t="shared" si="1"/>
         <v>456.41840436984171</v>
       </c>
     </row>
@@ -2292,7 +2292,7 @@
         <v>31.82</v>
       </c>
       <c r="H28" s="9">
-        <f>E28/G28</f>
+        <f t="shared" si="1"/>
         <v>304.83972344437461</v>
       </c>
       <c r="I28" t="s">
@@ -2314,9 +2314,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="16.375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.7109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.42578125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:14" x14ac:dyDescent="0.25">
@@ -2601,9 +2601,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.5703125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="18" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -3137,9 +3137,9 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.25" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="22.625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="15.28515625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="22.5703125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="14.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Found error in pH 5 pyrite calculation, reported masses in mg instead of g. Updated figures and SCM modeling for updated data.
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/Table1-KdValuesAndMineralProp.xlsx
+++ b/Manuscript/Tables/Table1-KdValuesAndMineralProp.xlsx
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="223" uniqueCount="70">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="221" uniqueCount="70">
   <si>
     <t>Mineral</t>
   </si>
@@ -502,11 +502,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="222917088"/>
-        <c:axId val="222919832"/>
+        <c:axId val="206712832"/>
+        <c:axId val="206706168"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="222917088"/>
+        <c:axId val="206712832"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -563,12 +563,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222919832"/>
+        <c:crossAx val="206706168"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="222919832"/>
+        <c:axId val="206706168"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -625,7 +625,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="222917088"/>
+        <c:crossAx val="206712832"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1531,7 +1531,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E13" sqref="E13"/>
+      <selection activeCell="G15" sqref="G15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1677,7 +1677,7 @@
         <v>9</v>
       </c>
       <c r="E6" s="10">
-        <v>115932.7</v>
+        <v>146111.69</v>
       </c>
       <c r="F6" s="10" t="s">
         <v>7</v>
@@ -1687,7 +1687,7 @@
       </c>
       <c r="H6" s="10">
         <f t="shared" si="0"/>
-        <v>302.77539827631239</v>
+        <v>381.59229563854797</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.25">
@@ -2030,8 +2030,8 @@
       <c r="D19" s="10">
         <v>3</v>
       </c>
-      <c r="E19" s="10" t="s">
-        <v>9</v>
+      <c r="E19" s="10">
+        <v>2969.14</v>
       </c>
       <c r="F19" s="10" t="s">
         <v>7</v>
@@ -2040,6 +2040,10 @@
         <f>AVERAGE(0.059,0.078)</f>
         <v>6.8500000000000005E-2</v>
       </c>
+      <c r="H19" s="10">
+        <f>E19/G19</f>
+        <v>43345.109489051087</v>
+      </c>
     </row>
     <row r="20" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="10" t="s">
@@ -2055,8 +2059,8 @@
       <c r="D20" s="10">
         <v>5</v>
       </c>
-      <c r="E20" s="10" t="s">
-        <v>9</v>
+      <c r="E20" s="10">
+        <v>3.52</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>7</v>
@@ -2065,6 +2069,10 @@
         <f>AVERAGE(0.059,0.078)</f>
         <v>6.8500000000000005E-2</v>
       </c>
+      <c r="H20" s="10">
+        <f>E20/G20</f>
+        <v>51.386861313868607</v>
+      </c>
     </row>
     <row r="21" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="10" t="s">
@@ -2081,7 +2089,7 @@
         <v>7</v>
       </c>
       <c r="E21" s="10">
-        <v>536</v>
+        <v>4007.12</v>
       </c>
       <c r="F21" s="10" t="s">
         <v>7</v>
@@ -2092,7 +2100,7 @@
       </c>
       <c r="H21" s="10">
         <f t="shared" ref="H21:H28" si="1">E21/G21</f>
-        <v>7824.8175182481746</v>
+        <v>58498.102189781013</v>
       </c>
     </row>
     <row r="22" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">
@@ -2110,7 +2118,7 @@
         <v>9</v>
       </c>
       <c r="E22" s="10">
-        <v>520</v>
+        <v>3674.09</v>
       </c>
       <c r="F22" s="10" t="s">
         <v>7</v>
@@ -2121,7 +2129,7 @@
       </c>
       <c r="H22" s="10">
         <f t="shared" si="1"/>
-        <v>7591.2408759124082</v>
+        <v>53636.350364963502</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
Mostly finished up reajdusting data for measurement error, though it is still unclear why that error happened in the first place. Additionally, blank sorption results are not making sense.
</commit_message>
<xml_diff>
--- a/Manuscript/Tables/Table1-KdValuesAndMineralProp.xlsx
+++ b/Manuscript/Tables/Table1-KdValuesAndMineralProp.xlsx
@@ -502,11 +502,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="206712832"/>
-        <c:axId val="206706168"/>
+        <c:axId val="198538640"/>
+        <c:axId val="198538248"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="206712832"/>
+        <c:axId val="198538640"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -563,12 +563,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206706168"/>
+        <c:crossAx val="198538248"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="206706168"/>
+        <c:axId val="198538248"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -625,7 +625,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="206712832"/>
+        <c:crossAx val="198538640"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1531,7 +1531,7 @@
   <dimension ref="A1:I28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G15" sqref="G15"/>
+      <selection activeCell="E13" sqref="E13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1841,7 +1841,7 @@
         <v>9</v>
       </c>
       <c r="E12" s="10">
-        <v>27975.15</v>
+        <v>26168.85</v>
       </c>
       <c r="F12" s="10" t="s">
         <v>7</v>
@@ -1851,7 +1851,7 @@
       </c>
       <c r="H12" s="10">
         <f>E12/G12</f>
-        <v>191.00880786562885</v>
+        <v>178.67574764440801</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.25">
@@ -2060,7 +2060,7 @@
         <v>5</v>
       </c>
       <c r="E20" s="10">
-        <v>3.52</v>
+        <v>3521.11</v>
       </c>
       <c r="F20" s="10" t="s">
         <v>7</v>
@@ -2071,7 +2071,7 @@
       </c>
       <c r="H20" s="10">
         <f>E20/G20</f>
-        <v>51.386861313868607</v>
+        <v>51403.065693430653</v>
       </c>
     </row>
     <row r="21" spans="1:9" s="10" customFormat="1" x14ac:dyDescent="0.25">

</xml_diff>